<commit_message>
Agregado de codigo y consulta del stock disponible
</commit_message>
<xml_diff>
--- a/Main/Index/Tabla_bulones.xlsx
+++ b/Main/Index/Tabla_bulones.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="194">
   <si>
     <t>godoyjorgedaniel@gmail.com</t>
   </si>
@@ -600,6 +600,15 @@
   </si>
   <si>
     <t>Identificador</t>
+  </si>
+  <si>
+    <t>Stock rosca der.</t>
+  </si>
+  <si>
+    <t>Stock rosca izq.</t>
+  </si>
+  <si>
+    <t>Diametro (mm)</t>
   </si>
 </sst>
 </file>
@@ -1457,21 +1466,24 @@
   <dimension ref="B1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="4" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="27" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>3</v>
@@ -1480,10 +1492,10 @@
         <v>16</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>1</v>
+        <v>192</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>2</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modificacion tabla y superdescriptores.
</commit_message>
<xml_diff>
--- a/Main/Index/Tabla_bulones.xlsx
+++ b/Main/Index/Tabla_bulones.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Stock" sheetId="4" r:id="rId1"/>
     <sheet name="Clientes" sheetId="1" r:id="rId2"/>
-    <sheet name="Stock-Base" sheetId="2" r:id="rId3"/>
+    <sheet name="Stock-Prog-Inicial" sheetId="2" r:id="rId3"/>
     <sheet name="Superdescriptores" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="403">
   <si>
     <t>godoyjorgedaniel@gmail.com</t>
   </si>
@@ -609,13 +609,640 @@
   </si>
   <si>
     <t>Diametro (mm)</t>
+  </si>
+  <si>
+    <t>06101401</t>
+  </si>
+  <si>
+    <t>06101201</t>
+  </si>
+  <si>
+    <t>06103401</t>
+  </si>
+  <si>
+    <t>06101001</t>
+  </si>
+  <si>
+    <t>07101401</t>
+  </si>
+  <si>
+    <t>07101201</t>
+  </si>
+  <si>
+    <t>07103401</t>
+  </si>
+  <si>
+    <t>07101001</t>
+  </si>
+  <si>
+    <t>08121401</t>
+  </si>
+  <si>
+    <t>08121201</t>
+  </si>
+  <si>
+    <t>08123401</t>
+  </si>
+  <si>
+    <t>08121001</t>
+  </si>
+  <si>
+    <t>09121401</t>
+  </si>
+  <si>
+    <t>09121201</t>
+  </si>
+  <si>
+    <t>09123401</t>
+  </si>
+  <si>
+    <t>0912101</t>
+  </si>
+  <si>
+    <t>10151401</t>
+  </si>
+  <si>
+    <t>10151201</t>
+  </si>
+  <si>
+    <t>10153401</t>
+  </si>
+  <si>
+    <t>16201401</t>
+  </si>
+  <si>
+    <t>16201201</t>
+  </si>
+  <si>
+    <t>16203401</t>
+  </si>
+  <si>
+    <t>16201001</t>
+  </si>
+  <si>
+    <t>18221401</t>
+  </si>
+  <si>
+    <t>18221201</t>
+  </si>
+  <si>
+    <t>18223401</t>
+  </si>
+  <si>
+    <t>18221001</t>
+  </si>
+  <si>
+    <t>20221401</t>
+  </si>
+  <si>
+    <t>20221201</t>
+  </si>
+  <si>
+    <t>20223401</t>
+  </si>
+  <si>
+    <t>20221001</t>
+  </si>
+  <si>
+    <t>22221401</t>
+  </si>
+  <si>
+    <t>22221201</t>
+  </si>
+  <si>
+    <t>22223401</t>
+  </si>
+  <si>
+    <t>22221001</t>
+  </si>
+  <si>
+    <t>24301401</t>
+  </si>
+  <si>
+    <t>24303401</t>
+  </si>
+  <si>
+    <t>24301001</t>
+  </si>
+  <si>
+    <t>27301401</t>
+  </si>
+  <si>
+    <t>27301201</t>
+  </si>
+  <si>
+    <t>27303401</t>
+  </si>
+  <si>
+    <t>27301001</t>
+  </si>
+  <si>
+    <t>30351401</t>
+  </si>
+  <si>
+    <t>30351201</t>
+  </si>
+  <si>
+    <t>30353401</t>
+  </si>
+  <si>
+    <t>30351001</t>
+  </si>
+  <si>
+    <t>33351401</t>
+  </si>
+  <si>
+    <t>33351201</t>
+  </si>
+  <si>
+    <t>33353401</t>
+  </si>
+  <si>
+    <t>33351001</t>
+  </si>
+  <si>
+    <t>36401401</t>
+  </si>
+  <si>
+    <t>36401201</t>
+  </si>
+  <si>
+    <t>36403401</t>
+  </si>
+  <si>
+    <t>36341001</t>
+  </si>
+  <si>
+    <t>39401401</t>
+  </si>
+  <si>
+    <t>39401201</t>
+  </si>
+  <si>
+    <t>39403401</t>
+  </si>
+  <si>
+    <t>39341001</t>
+  </si>
+  <si>
+    <t>42451401</t>
+  </si>
+  <si>
+    <t>42451201</t>
+  </si>
+  <si>
+    <t>42453401</t>
+  </si>
+  <si>
+    <t>42451001</t>
+  </si>
+  <si>
+    <t>45451401</t>
+  </si>
+  <si>
+    <t>45451201</t>
+  </si>
+  <si>
+    <t>45453401</t>
+  </si>
+  <si>
+    <t>45451001</t>
+  </si>
+  <si>
+    <t>48501401</t>
+  </si>
+  <si>
+    <t>48501201</t>
+  </si>
+  <si>
+    <t>48503401</t>
+  </si>
+  <si>
+    <t>48451001</t>
+  </si>
+  <si>
+    <t>52501401</t>
+  </si>
+  <si>
+    <t>52501201</t>
+  </si>
+  <si>
+    <t>52503401</t>
+  </si>
+  <si>
+    <t>52551001</t>
+  </si>
+  <si>
+    <t>56551401</t>
+  </si>
+  <si>
+    <t>56551201</t>
+  </si>
+  <si>
+    <t>56553401</t>
+  </si>
+  <si>
+    <t>56551001</t>
+  </si>
+  <si>
+    <t>60651401</t>
+  </si>
+  <si>
+    <t>60651201</t>
+  </si>
+  <si>
+    <t>60653401</t>
+  </si>
+  <si>
+    <t>60651001</t>
+  </si>
+  <si>
+    <t>64601401</t>
+  </si>
+  <si>
+    <t>64601201</t>
+  </si>
+  <si>
+    <t>64603401</t>
+  </si>
+  <si>
+    <t>64661001</t>
+  </si>
+  <si>
+    <t>68601401</t>
+  </si>
+  <si>
+    <t>68601201</t>
+  </si>
+  <si>
+    <t>68603401</t>
+  </si>
+  <si>
+    <t>68661001</t>
+  </si>
+  <si>
+    <t>72601401</t>
+  </si>
+  <si>
+    <t>72601201</t>
+  </si>
+  <si>
+    <t>72603401</t>
+  </si>
+  <si>
+    <t>72761001</t>
+  </si>
+  <si>
+    <t>76601401</t>
+  </si>
+  <si>
+    <t>76601201</t>
+  </si>
+  <si>
+    <t>76603401</t>
+  </si>
+  <si>
+    <t>76761001</t>
+  </si>
+  <si>
+    <t>80601401</t>
+  </si>
+  <si>
+    <t>80601201</t>
+  </si>
+  <si>
+    <t>80603401</t>
+  </si>
+  <si>
+    <t>80861001</t>
+  </si>
+  <si>
+    <t>10151001</t>
+  </si>
+  <si>
+    <t>06101400</t>
+  </si>
+  <si>
+    <t>06101200</t>
+  </si>
+  <si>
+    <t>06103400</t>
+  </si>
+  <si>
+    <t>06101000</t>
+  </si>
+  <si>
+    <t>07101400</t>
+  </si>
+  <si>
+    <t>07101200</t>
+  </si>
+  <si>
+    <t>07103400</t>
+  </si>
+  <si>
+    <t>07101000</t>
+  </si>
+  <si>
+    <t>08121400</t>
+  </si>
+  <si>
+    <t>08121200</t>
+  </si>
+  <si>
+    <t>08123400</t>
+  </si>
+  <si>
+    <t>08121000</t>
+  </si>
+  <si>
+    <t>09121400</t>
+  </si>
+  <si>
+    <t>09121200</t>
+  </si>
+  <si>
+    <t>09123400</t>
+  </si>
+  <si>
+    <t>09121000</t>
+  </si>
+  <si>
+    <t>10151400</t>
+  </si>
+  <si>
+    <t>10151200</t>
+  </si>
+  <si>
+    <t>10153400</t>
+  </si>
+  <si>
+    <t>10151000</t>
+  </si>
+  <si>
+    <t>16201400</t>
+  </si>
+  <si>
+    <t>16201200</t>
+  </si>
+  <si>
+    <t>16203400</t>
+  </si>
+  <si>
+    <t>16201000</t>
+  </si>
+  <si>
+    <t>18221400</t>
+  </si>
+  <si>
+    <t>18221200</t>
+  </si>
+  <si>
+    <t>18223400</t>
+  </si>
+  <si>
+    <t>18221000</t>
+  </si>
+  <si>
+    <t>20221400</t>
+  </si>
+  <si>
+    <t>20221200</t>
+  </si>
+  <si>
+    <t>20223400</t>
+  </si>
+  <si>
+    <t>20221000</t>
+  </si>
+  <si>
+    <t>22221400</t>
+  </si>
+  <si>
+    <t>22221200</t>
+  </si>
+  <si>
+    <t>22223400</t>
+  </si>
+  <si>
+    <t>22221000</t>
+  </si>
+  <si>
+    <t>24301400</t>
+  </si>
+  <si>
+    <t>24303400</t>
+  </si>
+  <si>
+    <t>24301000</t>
+  </si>
+  <si>
+    <t>27301400</t>
+  </si>
+  <si>
+    <t>27301200</t>
+  </si>
+  <si>
+    <t>27303400</t>
+  </si>
+  <si>
+    <t>27301000</t>
+  </si>
+  <si>
+    <t>30351400</t>
+  </si>
+  <si>
+    <t>30351200</t>
+  </si>
+  <si>
+    <t>30353400</t>
+  </si>
+  <si>
+    <t>30351000</t>
+  </si>
+  <si>
+    <t>33351400</t>
+  </si>
+  <si>
+    <t>33351200</t>
+  </si>
+  <si>
+    <t>33353400</t>
+  </si>
+  <si>
+    <t>33351000</t>
+  </si>
+  <si>
+    <t>36401400</t>
+  </si>
+  <si>
+    <t>36401200</t>
+  </si>
+  <si>
+    <t>36403400</t>
+  </si>
+  <si>
+    <t>36341000</t>
+  </si>
+  <si>
+    <t>39401400</t>
+  </si>
+  <si>
+    <t>39401200</t>
+  </si>
+  <si>
+    <t>39403400</t>
+  </si>
+  <si>
+    <t>39341000</t>
+  </si>
+  <si>
+    <t>42451400</t>
+  </si>
+  <si>
+    <t>42451200</t>
+  </si>
+  <si>
+    <t>42453400</t>
+  </si>
+  <si>
+    <t>42451000</t>
+  </si>
+  <si>
+    <t>45451400</t>
+  </si>
+  <si>
+    <t>45451200</t>
+  </si>
+  <si>
+    <t>45453400</t>
+  </si>
+  <si>
+    <t>45451000</t>
+  </si>
+  <si>
+    <t>48501400</t>
+  </si>
+  <si>
+    <t>48501200</t>
+  </si>
+  <si>
+    <t>48503400</t>
+  </si>
+  <si>
+    <t>48451000</t>
+  </si>
+  <si>
+    <t>52501400</t>
+  </si>
+  <si>
+    <t>52501200</t>
+  </si>
+  <si>
+    <t>52503400</t>
+  </si>
+  <si>
+    <t>52551000</t>
+  </si>
+  <si>
+    <t>56551400</t>
+  </si>
+  <si>
+    <t>56551200</t>
+  </si>
+  <si>
+    <t>56553400</t>
+  </si>
+  <si>
+    <t>56551000</t>
+  </si>
+  <si>
+    <t>60651400</t>
+  </si>
+  <si>
+    <t>60651200</t>
+  </si>
+  <si>
+    <t>60653400</t>
+  </si>
+  <si>
+    <t>60651000</t>
+  </si>
+  <si>
+    <t>64601400</t>
+  </si>
+  <si>
+    <t>64601200</t>
+  </si>
+  <si>
+    <t>64603400</t>
+  </si>
+  <si>
+    <t>64661000</t>
+  </si>
+  <si>
+    <t>68601400</t>
+  </si>
+  <si>
+    <t>68601200</t>
+  </si>
+  <si>
+    <t>68603400</t>
+  </si>
+  <si>
+    <t>68661000</t>
+  </si>
+  <si>
+    <t>72601400</t>
+  </si>
+  <si>
+    <t>72601200</t>
+  </si>
+  <si>
+    <t>72603400</t>
+  </si>
+  <si>
+    <t>72761000</t>
+  </si>
+  <si>
+    <t>76601400</t>
+  </si>
+  <si>
+    <t>76601200</t>
+  </si>
+  <si>
+    <t>76603400</t>
+  </si>
+  <si>
+    <t>76761000</t>
+  </si>
+  <si>
+    <t>80601400</t>
+  </si>
+  <si>
+    <t>80601200</t>
+  </si>
+  <si>
+    <t>80603400</t>
+  </si>
+  <si>
+    <t>80861000</t>
+  </si>
+  <si>
+    <t>NOTA: Superdescriptores para la version de prueba en los comienzos del probrama Bulones0A</t>
+  </si>
+  <si>
+    <t>Superdescriptor SRD</t>
+  </si>
+  <si>
+    <t>Superdescriptor SRI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,6 +1260,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -664,7 +1299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -973,12 +1608,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1064,9 +1712,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1076,9 +1721,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1088,9 +1730,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1100,9 +1739,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1112,9 +1748,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1124,9 +1757,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1147,6 +1777,48 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1463,10 +2135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F106"/>
+  <dimension ref="B1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,13 +2147,15 @@
     <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="4" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="27" t="s">
         <v>193</v>
       </c>
@@ -1491,14 +2165,20 @@
       <c r="D2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>401</v>
+      </c>
+      <c r="G2" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="11" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="30">
         <v>6</v>
       </c>
@@ -1508,133 +2188,181 @@
       <c r="D3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="56">
+        <v>5500</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="G3" s="31">
         <v>1000</v>
       </c>
-      <c r="F3" s="33">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="34">
+      <c r="H3" s="57" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="33">
         <v>6</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="34">
         <v>1</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="58">
+        <v>2800</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="G4" s="34">
         <v>1500</v>
       </c>
-      <c r="F4" s="37">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="34">
+      <c r="H4" s="59" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="33">
         <v>6</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="34">
         <v>1</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="58">
+        <v>5600</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="G5" s="34">
         <v>2000</v>
       </c>
-      <c r="F5" s="37">
-        <v>5600</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="38">
+      <c r="H5" s="59" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="36">
         <v>6</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="37">
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="60">
+        <v>2900</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="G6" s="37">
         <v>2500</v>
       </c>
-      <c r="F6" s="41">
-        <v>2900</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="42">
+      <c r="H6" s="61" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="39">
         <v>7</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="40">
         <v>1</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="62">
+        <v>2950</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="G7" s="40">
         <v>1100</v>
       </c>
-      <c r="F7" s="45">
-        <v>2950</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="46">
+      <c r="H7" s="63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="42">
         <v>7</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="43">
         <v>1</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="64">
+        <v>2450</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="G8" s="43">
         <v>1600</v>
       </c>
-      <c r="F8" s="49">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="46">
+      <c r="H8" s="65" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="42">
         <v>7</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="43">
         <v>1</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="64">
+        <v>1950</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>303</v>
+      </c>
+      <c r="G9" s="43">
         <v>2000</v>
       </c>
-      <c r="F9" s="49">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="50">
+      <c r="H9" s="65" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="45">
         <v>7</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="46">
         <v>1</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="66">
+        <v>1450</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>304</v>
+      </c>
+      <c r="G10" s="46">
         <v>2600</v>
       </c>
-      <c r="F10" s="53">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="67" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="30">
         <v>8</v>
       </c>
@@ -1644,133 +2372,181 @@
       <c r="D11" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="56">
+        <v>5500</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="G11" s="31">
         <v>1200</v>
       </c>
-      <c r="F11" s="33">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="34">
+      <c r="H11" s="57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="33">
         <v>8</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="58">
+        <v>2800</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="G12" s="34">
         <v>1700</v>
       </c>
-      <c r="F12" s="37">
+      <c r="H12" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="33">
+        <v>8</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="58">
+        <v>5600</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="G13" s="34">
+        <v>2200</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="36">
+        <v>8</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="60">
+        <v>2900</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>308</v>
+      </c>
+      <c r="G14" s="37">
+        <v>2700</v>
+      </c>
+      <c r="H14" s="61" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="39">
+        <v>9</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="62">
+        <v>2950</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="40">
+        <v>1300</v>
+      </c>
+      <c r="H15" s="63" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="42">
+        <v>9</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="64">
+        <v>2450</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="G16" s="43">
+        <v>1800</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="42">
+        <v>9</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="64">
+        <v>1950</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="G17" s="43">
+        <v>2300</v>
+      </c>
+      <c r="H17" s="65" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="45">
+        <v>9</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="66">
+        <v>1450</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>312</v>
+      </c>
+      <c r="G18" s="46">
         <v>2800</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="34">
-        <v>8</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="35">
-        <v>2200</v>
-      </c>
-      <c r="F13" s="37">
-        <v>5600</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="38">
-        <v>8</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="39">
-        <v>2700</v>
-      </c>
-      <c r="F14" s="41">
-        <v>2900</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="42">
-        <v>9</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="43">
-        <v>1300</v>
-      </c>
-      <c r="F15" s="45">
-        <v>2950</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="46">
-        <v>9</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="47">
-        <v>1800</v>
-      </c>
-      <c r="F16" s="49">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="46">
-        <v>9</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="47">
-        <v>2300</v>
-      </c>
-      <c r="F17" s="49">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="50">
-        <v>9</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="51">
-        <v>2800</v>
-      </c>
-      <c r="F18" s="53">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="67" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="30">
         <v>10</v>
       </c>
@@ -1780,133 +2556,181 @@
       <c r="D19" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="56">
+        <v>6000</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="G19" s="31">
         <v>1000</v>
       </c>
-      <c r="F19" s="33">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="34">
+      <c r="H19" s="57" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="33">
         <v>10</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="58">
+        <v>6300</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="G20" s="34">
         <v>1500</v>
       </c>
-      <c r="F20" s="37">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="34">
+      <c r="H20" s="59" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="33">
         <v>10</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="58">
+        <v>6600</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="G21" s="34">
         <v>2000</v>
       </c>
-      <c r="F21" s="37">
-        <v>6600</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="38">
+      <c r="H21" s="59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="36">
         <v>10</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="39">
+      <c r="E22" s="60">
+        <v>6900</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="G22" s="37">
         <v>2500</v>
       </c>
-      <c r="F22" s="41">
-        <v>6900</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="42">
+      <c r="H22" s="61" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="39">
         <v>16</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="40">
         <v>2</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="62">
+        <v>7200</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="G23" s="40">
         <v>1100</v>
       </c>
-      <c r="F23" s="45">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="46">
+      <c r="H23" s="63" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="42">
         <v>16</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="43">
         <v>2</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="47">
+      <c r="E24" s="64">
+        <v>7500</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="G24" s="43">
         <v>1600</v>
       </c>
-      <c r="F24" s="49">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="46">
+      <c r="H24" s="65" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="42">
         <v>16</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="43">
         <v>2</v>
       </c>
-      <c r="D25" s="48" t="s">
+      <c r="D25" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="47">
+      <c r="E25" s="64">
+        <v>7800</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="G25" s="43">
         <v>2000</v>
       </c>
-      <c r="F25" s="49">
-        <v>7800</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="50">
+      <c r="H25" s="65" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="45">
         <v>16</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="46">
         <v>2</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="51">
+      <c r="E26" s="66">
+        <v>8100</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="G26" s="46">
         <v>2600</v>
       </c>
-      <c r="F26" s="53">
-        <v>8100</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H26" s="67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="30">
         <v>18</v>
       </c>
@@ -1916,133 +2740,181 @@
       <c r="D27" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="56">
+        <v>8600</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="G27" s="31">
         <v>1200</v>
       </c>
-      <c r="F27" s="33">
-        <v>8600</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="34">
+      <c r="H27" s="57" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="33">
         <v>18</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="35">
+      <c r="E28" s="58">
+        <v>8400</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="G28" s="34">
         <v>1700</v>
       </c>
-      <c r="F28" s="37">
-        <v>8400</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="34">
+      <c r="H28" s="59" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="33">
         <v>18</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="58">
+        <v>8200</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>323</v>
+      </c>
+      <c r="G29" s="34">
         <v>2200</v>
       </c>
-      <c r="F29" s="37">
-        <v>8200</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="38">
+      <c r="H29" s="59" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="36">
         <v>18</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="39">
+      <c r="E30" s="60">
+        <v>8000</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="G30" s="37">
         <v>2700</v>
       </c>
-      <c r="F30" s="41">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="42">
+      <c r="H30" s="61" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="39">
         <v>20</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="62">
+        <v>7800</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="G31" s="40">
         <v>1300</v>
       </c>
-      <c r="F31" s="45">
-        <v>7800</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="46">
+      <c r="H31" s="63" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="42">
         <v>20</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="47">
+      <c r="E32" s="64">
+        <v>7600</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="G32" s="43">
         <v>1800</v>
       </c>
-      <c r="F32" s="49">
-        <v>7600</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="46">
+      <c r="H32" s="65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="42">
         <v>20</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="48" t="s">
+      <c r="D33" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="47">
+      <c r="E33" s="64">
+        <v>7400</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="G33" s="43">
         <v>2300</v>
       </c>
-      <c r="F33" s="49">
-        <v>7400</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="50">
+      <c r="H33" s="65" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="45">
         <v>20</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="51">
+      <c r="E34" s="66">
+        <v>7200</v>
+      </c>
+      <c r="F34" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="G34" s="46">
         <v>2800</v>
       </c>
-      <c r="F34" s="53">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H34" s="67" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="30">
         <v>22</v>
       </c>
@@ -2052,133 +2924,181 @@
       <c r="D35" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="56">
+        <v>7000</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="G35" s="31">
         <v>1000</v>
       </c>
-      <c r="F35" s="33">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="34">
+      <c r="H35" s="57" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="33">
         <v>22</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="58">
+        <v>6800</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="G36" s="34">
         <v>1500</v>
       </c>
-      <c r="F36" s="37">
-        <v>6800</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="34">
+      <c r="H36" s="59" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="33">
         <v>22</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="35">
+      <c r="E37" s="58">
+        <v>6600</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="G37" s="34">
         <v>2000</v>
       </c>
-      <c r="F37" s="37">
-        <v>6600</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="38">
+      <c r="H37" s="59" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="36">
         <v>22</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="40" t="s">
+      <c r="D38" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="39">
+      <c r="E38" s="60">
+        <v>6400</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="G38" s="37">
         <v>2500</v>
       </c>
-      <c r="F38" s="41">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="42">
+      <c r="H38" s="61" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="39">
         <v>24</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="40">
         <v>3</v>
       </c>
-      <c r="D39" s="44" t="s">
+      <c r="D39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="62">
+        <v>7100</v>
+      </c>
+      <c r="F39" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="G39" s="40">
         <v>1100</v>
       </c>
-      <c r="F39" s="45">
-        <v>7100</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="46">
+      <c r="H39" s="63" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="42">
         <v>24</v>
       </c>
-      <c r="C40" s="47">
+      <c r="C40" s="43">
         <v>3</v>
       </c>
-      <c r="D40" s="48" t="s">
+      <c r="D40" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="47">
+      <c r="E40" s="64">
+        <v>7350</v>
+      </c>
+      <c r="F40" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="G40" s="43">
         <v>1600</v>
       </c>
-      <c r="F40" s="49">
-        <v>7350</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="46">
+      <c r="H40" s="65" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="42">
         <v>24</v>
       </c>
-      <c r="C41" s="47">
+      <c r="C41" s="43">
         <v>3</v>
       </c>
-      <c r="D41" s="48" t="s">
+      <c r="D41" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="47">
+      <c r="E41" s="64">
+        <v>7600</v>
+      </c>
+      <c r="F41" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="G41" s="43">
         <v>2000</v>
       </c>
-      <c r="F41" s="49">
-        <v>7600</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="50">
+      <c r="H41" s="65" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="45">
         <v>24</v>
       </c>
-      <c r="C42" s="51">
+      <c r="C42" s="46">
         <v>3</v>
       </c>
-      <c r="D42" s="52" t="s">
+      <c r="D42" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="51">
+      <c r="E42" s="66">
+        <v>7850</v>
+      </c>
+      <c r="F42" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="G42" s="46">
         <v>2600</v>
       </c>
-      <c r="F42" s="53">
-        <v>7850</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H42" s="67" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="30">
         <v>27</v>
       </c>
@@ -2188,133 +3108,181 @@
       <c r="D43" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="31">
+      <c r="E43" s="56">
+        <v>8100</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="G43" s="31">
         <v>1200</v>
       </c>
-      <c r="F43" s="33">
-        <v>8100</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="34">
+      <c r="H43" s="57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="33">
         <v>27</v>
       </c>
-      <c r="C44" s="35">
+      <c r="C44" s="34">
         <v>3</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="35">
+      <c r="E44" s="58">
+        <v>8350</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="G44" s="34">
         <v>1700</v>
       </c>
-      <c r="F44" s="37">
-        <v>8350</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="34">
+      <c r="H44" s="59" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="33">
         <v>27</v>
       </c>
-      <c r="C45" s="35">
+      <c r="C45" s="34">
         <v>3</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D45" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="35">
+      <c r="E45" s="58">
+        <v>8600</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="G45" s="34">
         <v>2200</v>
       </c>
-      <c r="F45" s="37">
-        <v>8600</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="38">
+      <c r="H45" s="59" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="36">
         <v>27</v>
       </c>
-      <c r="C46" s="39">
+      <c r="C46" s="37">
         <v>3</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="39">
+      <c r="E46" s="60">
+        <v>8850</v>
+      </c>
+      <c r="F46" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="G46" s="37">
         <v>2700</v>
       </c>
-      <c r="F46" s="41">
-        <v>8850</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="42">
+      <c r="H46" s="61" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="39">
         <v>30</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="43">
+      <c r="E47" s="62">
+        <v>9100</v>
+      </c>
+      <c r="F47" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="G47" s="40">
         <v>1300</v>
       </c>
-      <c r="F47" s="45">
+      <c r="H47" s="63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="42">
+        <v>30</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="64">
+        <v>9150</v>
+      </c>
+      <c r="F48" s="44" t="s">
+        <v>341</v>
+      </c>
+      <c r="G48" s="43">
+        <v>1800</v>
+      </c>
+      <c r="H48" s="65" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="42">
+        <v>30</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="64">
         <v>9100</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="46">
+      <c r="F49" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="G49" s="43">
+        <v>2300</v>
+      </c>
+      <c r="H49" s="65" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="45">
         <v>30</v>
       </c>
-      <c r="C48" s="47" t="s">
+      <c r="C50" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="47">
-        <v>1800</v>
-      </c>
-      <c r="F48" s="49">
-        <v>9150</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="46">
-        <v>30</v>
-      </c>
-      <c r="C49" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="E49" s="47">
-        <v>2300</v>
-      </c>
-      <c r="F49" s="49">
-        <v>9100</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="50">
-        <v>30</v>
-      </c>
-      <c r="C50" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="52" t="s">
+      <c r="D50" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="51">
+      <c r="E50" s="66">
+        <v>9050</v>
+      </c>
+      <c r="F50" s="47" t="s">
+        <v>343</v>
+      </c>
+      <c r="G50" s="46">
         <v>2800</v>
       </c>
-      <c r="F50" s="53">
-        <v>9050</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H50" s="67" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="30">
         <v>33</v>
       </c>
@@ -2324,133 +3292,181 @@
       <c r="D51" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="31">
+      <c r="E51" s="56">
+        <v>9000</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>344</v>
+      </c>
+      <c r="G51" s="31">
         <v>1000</v>
       </c>
-      <c r="F51" s="33">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="34">
+      <c r="H51" s="57" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="33">
         <v>33</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="35">
+      <c r="E52" s="58">
+        <v>8950</v>
+      </c>
+      <c r="F52" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="G52" s="34">
         <v>1500</v>
       </c>
-      <c r="F52" s="37">
-        <v>8950</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="34">
+      <c r="H52" s="59" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="33">
         <v>33</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="36" t="s">
+      <c r="D53" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="35">
+      <c r="E53" s="58">
+        <v>8900</v>
+      </c>
+      <c r="F53" s="35" t="s">
+        <v>346</v>
+      </c>
+      <c r="G53" s="34">
         <v>2000</v>
       </c>
-      <c r="F53" s="37">
-        <v>8900</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="38">
+      <c r="H53" s="59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="36">
         <v>33</v>
       </c>
-      <c r="C54" s="39" t="s">
+      <c r="C54" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="40" t="s">
+      <c r="D54" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="39">
+      <c r="E54" s="60">
+        <v>8850</v>
+      </c>
+      <c r="F54" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="G54" s="37">
         <v>2500</v>
       </c>
-      <c r="F54" s="41">
-        <v>8850</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="42">
+      <c r="H54" s="61" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="39">
         <v>36</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="40">
         <v>4</v>
       </c>
-      <c r="D55" s="44" t="s">
+      <c r="D55" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="43">
+      <c r="E55" s="62">
+        <v>8800</v>
+      </c>
+      <c r="F55" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="G55" s="40">
         <v>1100</v>
       </c>
-      <c r="F55" s="45">
-        <v>8800</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="46">
+      <c r="H55" s="63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="42">
         <v>36</v>
       </c>
-      <c r="C56" s="47">
+      <c r="C56" s="43">
         <v>4</v>
       </c>
-      <c r="D56" s="48" t="s">
+      <c r="D56" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="47">
+      <c r="E56" s="64">
+        <v>8750</v>
+      </c>
+      <c r="F56" s="44" t="s">
+        <v>349</v>
+      </c>
+      <c r="G56" s="43">
         <v>1600</v>
       </c>
-      <c r="F56" s="49">
-        <v>8750</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="46">
+      <c r="H56" s="65" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="42">
         <v>36</v>
       </c>
-      <c r="C57" s="47">
+      <c r="C57" s="43">
         <v>4</v>
       </c>
-      <c r="D57" s="48" t="s">
+      <c r="D57" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E57" s="47">
+      <c r="E57" s="64">
+        <v>8700</v>
+      </c>
+      <c r="F57" s="44" t="s">
+        <v>350</v>
+      </c>
+      <c r="G57" s="43">
         <v>2000</v>
       </c>
-      <c r="F57" s="49">
-        <v>8700</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="50">
+      <c r="H57" s="65" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="45">
         <v>36</v>
       </c>
-      <c r="C58" s="51">
+      <c r="C58" s="46">
         <v>4</v>
       </c>
-      <c r="D58" s="52" t="s">
+      <c r="D58" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="51">
+      <c r="E58" s="66">
+        <v>8650</v>
+      </c>
+      <c r="F58" s="47" t="s">
+        <v>351</v>
+      </c>
+      <c r="G58" s="46">
         <v>2600</v>
       </c>
-      <c r="F58" s="53">
-        <v>8650</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H58" s="67" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="30">
         <v>39</v>
       </c>
@@ -2460,133 +3476,181 @@
       <c r="D59" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="31">
+      <c r="E59" s="56">
+        <v>8600</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="G59" s="31">
         <v>1200</v>
       </c>
-      <c r="F59" s="33">
-        <v>8600</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="34">
+      <c r="H59" s="57" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="33">
         <v>39</v>
       </c>
-      <c r="C60" s="35">
+      <c r="C60" s="34">
         <v>4</v>
       </c>
-      <c r="D60" s="36" t="s">
+      <c r="D60" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="35">
+      <c r="E60" s="58">
+        <v>8550</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>353</v>
+      </c>
+      <c r="G60" s="34">
         <v>1700</v>
       </c>
-      <c r="F60" s="37">
-        <v>8550</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="34">
+      <c r="H60" s="59" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="33">
         <v>39</v>
       </c>
-      <c r="C61" s="35">
+      <c r="C61" s="34">
         <v>4</v>
       </c>
-      <c r="D61" s="36" t="s">
+      <c r="D61" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E61" s="35">
+      <c r="E61" s="58">
+        <v>8500</v>
+      </c>
+      <c r="F61" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="G61" s="34">
         <v>2200</v>
       </c>
-      <c r="F61" s="37">
-        <v>8500</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="38">
+      <c r="H61" s="59" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="36">
         <v>39</v>
       </c>
-      <c r="C62" s="39">
+      <c r="C62" s="37">
         <v>4</v>
       </c>
-      <c r="D62" s="40" t="s">
+      <c r="D62" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="39">
+      <c r="E62" s="60">
+        <v>8450</v>
+      </c>
+      <c r="F62" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="G62" s="37">
         <v>2700</v>
       </c>
-      <c r="F62" s="41">
-        <v>8450</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="42">
+      <c r="H62" s="61" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="39">
         <v>42</v>
       </c>
-      <c r="C63" s="43" t="s">
+      <c r="C63" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D63" s="44" t="s">
+      <c r="D63" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E63" s="43">
+      <c r="E63" s="62">
+        <v>9800</v>
+      </c>
+      <c r="F63" s="41" t="s">
+        <v>356</v>
+      </c>
+      <c r="G63" s="40">
         <v>1300</v>
       </c>
-      <c r="F63" s="45">
-        <v>9800</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="46">
+      <c r="H63" s="63" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="42">
         <v>42</v>
       </c>
-      <c r="C64" s="47" t="s">
+      <c r="C64" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D64" s="48" t="s">
+      <c r="D64" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="47">
+      <c r="E64" s="64">
+        <v>9805</v>
+      </c>
+      <c r="F64" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="G64" s="43">
         <v>1800</v>
       </c>
-      <c r="F64" s="49">
-        <v>9805</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="46">
+      <c r="H64" s="65" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="42">
         <v>42</v>
       </c>
-      <c r="C65" s="47" t="s">
+      <c r="C65" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D65" s="48" t="s">
+      <c r="D65" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E65" s="47">
+      <c r="E65" s="64">
+        <v>9810</v>
+      </c>
+      <c r="F65" s="44" t="s">
+        <v>358</v>
+      </c>
+      <c r="G65" s="43">
         <v>2300</v>
       </c>
-      <c r="F65" s="49">
-        <v>9810</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="50">
+      <c r="H65" s="65" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="45">
         <v>42</v>
       </c>
-      <c r="C66" s="51" t="s">
+      <c r="C66" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="52" t="s">
+      <c r="D66" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E66" s="51">
+      <c r="E66" s="66">
+        <v>9815</v>
+      </c>
+      <c r="F66" s="47" t="s">
+        <v>359</v>
+      </c>
+      <c r="G66" s="46">
         <v>2800</v>
       </c>
-      <c r="F66" s="53">
-        <v>9815</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H66" s="67" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="30">
         <v>45</v>
       </c>
@@ -2596,133 +3660,181 @@
       <c r="D67" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E67" s="31">
+      <c r="E67" s="56">
+        <v>9820</v>
+      </c>
+      <c r="F67" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="G67" s="31">
         <v>1000</v>
       </c>
-      <c r="F67" s="33">
-        <v>9820</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="34">
+      <c r="H67" s="57" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="33">
         <v>45</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C68" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="36" t="s">
+      <c r="D68" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E68" s="35">
+      <c r="E68" s="58">
+        <v>9825</v>
+      </c>
+      <c r="F68" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="G68" s="34">
         <v>1500</v>
       </c>
-      <c r="F68" s="37">
-        <v>9825</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="34">
+      <c r="H68" s="59" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="33">
         <v>45</v>
       </c>
-      <c r="C69" s="35" t="s">
+      <c r="C69" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="36" t="s">
+      <c r="D69" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E69" s="35">
+      <c r="E69" s="58">
+        <v>9830</v>
+      </c>
+      <c r="F69" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="G69" s="34">
         <v>2000</v>
       </c>
-      <c r="F69" s="37">
-        <v>9830</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="38">
+      <c r="H69" s="59" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="36">
         <v>45</v>
       </c>
-      <c r="C70" s="39" t="s">
+      <c r="C70" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="40" t="s">
+      <c r="D70" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E70" s="39">
+      <c r="E70" s="60">
+        <v>9835</v>
+      </c>
+      <c r="F70" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="G70" s="37">
         <v>2500</v>
       </c>
-      <c r="F70" s="41">
-        <v>9835</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="42">
+      <c r="H70" s="61" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="39">
         <v>48</v>
       </c>
-      <c r="C71" s="43">
+      <c r="C71" s="40">
         <v>5</v>
       </c>
-      <c r="D71" s="44" t="s">
+      <c r="D71" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="43">
+      <c r="E71" s="62">
+        <v>9840</v>
+      </c>
+      <c r="F71" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="G71" s="40">
         <v>1100</v>
       </c>
-      <c r="F71" s="45">
-        <v>9840</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="46">
+      <c r="H71" s="63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="42">
         <v>48</v>
       </c>
-      <c r="C72" s="47">
+      <c r="C72" s="43">
         <v>5</v>
       </c>
-      <c r="D72" s="48" t="s">
+      <c r="D72" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="47">
+      <c r="E72" s="64">
+        <v>9845</v>
+      </c>
+      <c r="F72" s="44" t="s">
+        <v>365</v>
+      </c>
+      <c r="G72" s="43">
         <v>1600</v>
       </c>
-      <c r="F72" s="49">
-        <v>9845</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="46">
+      <c r="H72" s="65" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="42">
         <v>48</v>
       </c>
-      <c r="C73" s="47">
+      <c r="C73" s="43">
         <v>5</v>
       </c>
-      <c r="D73" s="48" t="s">
+      <c r="D73" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E73" s="47">
+      <c r="E73" s="64">
+        <v>9850</v>
+      </c>
+      <c r="F73" s="44" t="s">
+        <v>366</v>
+      </c>
+      <c r="G73" s="43">
         <v>2000</v>
       </c>
-      <c r="F73" s="49">
-        <v>9850</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="50">
+      <c r="H73" s="65" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="45">
         <v>48</v>
       </c>
-      <c r="C74" s="51">
+      <c r="C74" s="46">
         <v>5</v>
       </c>
-      <c r="D74" s="52" t="s">
+      <c r="D74" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E74" s="51">
+      <c r="E74" s="66">
+        <v>9855</v>
+      </c>
+      <c r="F74" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="G74" s="46">
         <v>2600</v>
       </c>
-      <c r="F74" s="53">
-        <v>9855</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H74" s="67" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="30">
         <v>52</v>
       </c>
@@ -2732,133 +3844,181 @@
       <c r="D75" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E75" s="31">
+      <c r="E75" s="56">
+        <v>9860</v>
+      </c>
+      <c r="F75" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="G75" s="31">
         <v>1200</v>
       </c>
-      <c r="F75" s="33">
-        <v>9860</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="34">
+      <c r="H75" s="57" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="33">
         <v>52</v>
       </c>
-      <c r="C76" s="35">
+      <c r="C76" s="34">
         <v>5</v>
       </c>
-      <c r="D76" s="36" t="s">
+      <c r="D76" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E76" s="35">
+      <c r="E76" s="58">
+        <v>9865</v>
+      </c>
+      <c r="F76" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="G76" s="34">
         <v>1700</v>
       </c>
-      <c r="F76" s="37">
-        <v>9865</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="34">
+      <c r="H76" s="59" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="33">
         <v>52</v>
       </c>
-      <c r="C77" s="35">
+      <c r="C77" s="34">
         <v>5</v>
       </c>
-      <c r="D77" s="36" t="s">
+      <c r="D77" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E77" s="35">
+      <c r="E77" s="58">
+        <v>9870</v>
+      </c>
+      <c r="F77" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="G77" s="34">
         <v>2200</v>
       </c>
-      <c r="F77" s="37">
-        <v>9870</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="38">
+      <c r="H77" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="36">
         <v>52</v>
       </c>
-      <c r="C78" s="39">
+      <c r="C78" s="37">
         <v>5</v>
       </c>
-      <c r="D78" s="40" t="s">
+      <c r="D78" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E78" s="39">
+      <c r="E78" s="60">
+        <v>9875</v>
+      </c>
+      <c r="F78" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="G78" s="37">
         <v>2700</v>
       </c>
-      <c r="F78" s="41">
-        <v>9875</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="42">
+      <c r="H78" s="61" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="39">
         <v>56</v>
       </c>
-      <c r="C79" s="43" t="s">
+      <c r="C79" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D79" s="44" t="s">
+      <c r="D79" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E79" s="43">
+      <c r="E79" s="62">
+        <v>9880</v>
+      </c>
+      <c r="F79" s="41" t="s">
+        <v>372</v>
+      </c>
+      <c r="G79" s="40">
         <v>1300</v>
       </c>
-      <c r="F79" s="45">
-        <v>9880</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="46">
+      <c r="H79" s="63" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="42">
         <v>56</v>
       </c>
-      <c r="C80" s="47" t="s">
+      <c r="C80" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D80" s="48" t="s">
+      <c r="D80" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E80" s="47">
+      <c r="E80" s="64">
+        <v>9885</v>
+      </c>
+      <c r="F80" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="G80" s="43">
         <v>1800</v>
       </c>
-      <c r="F80" s="49">
-        <v>9885</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="46">
+      <c r="H80" s="65" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="42">
         <v>56</v>
       </c>
-      <c r="C81" s="47" t="s">
+      <c r="C81" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D81" s="48" t="s">
+      <c r="D81" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E81" s="47">
+      <c r="E81" s="64">
+        <v>9890</v>
+      </c>
+      <c r="F81" s="44" t="s">
+        <v>374</v>
+      </c>
+      <c r="G81" s="43">
         <v>2300</v>
       </c>
-      <c r="F81" s="49">
-        <v>9890</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="50">
+      <c r="H81" s="65" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="45">
         <v>56</v>
       </c>
-      <c r="C82" s="51" t="s">
+      <c r="C82" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D82" s="52" t="s">
+      <c r="D82" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E82" s="51">
+      <c r="E82" s="66">
+        <v>9895</v>
+      </c>
+      <c r="F82" s="47" t="s">
+        <v>375</v>
+      </c>
+      <c r="G82" s="46">
         <v>2800</v>
       </c>
-      <c r="F82" s="53">
-        <v>9895</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H82" s="67" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="30">
         <v>60</v>
       </c>
@@ -2868,133 +4028,181 @@
       <c r="D83" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="31">
+      <c r="E83" s="56">
+        <v>9900</v>
+      </c>
+      <c r="F83" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="G83" s="31">
         <v>1000</v>
       </c>
-      <c r="F83" s="33">
-        <v>9900</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84" s="34">
+      <c r="H83" s="57" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="33">
         <v>60</v>
       </c>
-      <c r="C84" s="35" t="s">
+      <c r="C84" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D84" s="36" t="s">
+      <c r="D84" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E84" s="35">
+      <c r="E84" s="58">
+        <v>9905</v>
+      </c>
+      <c r="F84" s="35" t="s">
+        <v>377</v>
+      </c>
+      <c r="G84" s="34">
         <v>1500</v>
       </c>
-      <c r="F84" s="37">
-        <v>9905</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B85" s="34">
+      <c r="H84" s="59" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="33">
         <v>60</v>
       </c>
-      <c r="C85" s="35" t="s">
+      <c r="C85" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D85" s="36" t="s">
+      <c r="D85" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E85" s="35">
+      <c r="E85" s="58">
+        <v>9910</v>
+      </c>
+      <c r="F85" s="35" t="s">
+        <v>378</v>
+      </c>
+      <c r="G85" s="34">
         <v>2000</v>
       </c>
-      <c r="F85" s="37">
-        <v>9910</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="38">
+      <c r="H85" s="59" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="36">
         <v>60</v>
       </c>
-      <c r="C86" s="39" t="s">
+      <c r="C86" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D86" s="40" t="s">
+      <c r="D86" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E86" s="39">
+      <c r="E86" s="60">
+        <v>9915</v>
+      </c>
+      <c r="F86" s="38" t="s">
+        <v>379</v>
+      </c>
+      <c r="G86" s="37">
         <v>2500</v>
       </c>
-      <c r="F86" s="41">
-        <v>9915</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="42">
+      <c r="H86" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="39">
         <v>64</v>
       </c>
-      <c r="C87" s="43">
+      <c r="C87" s="40">
         <v>6</v>
       </c>
-      <c r="D87" s="44" t="s">
+      <c r="D87" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E87" s="43">
+      <c r="E87" s="62">
+        <v>9950</v>
+      </c>
+      <c r="F87" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="G87" s="40">
         <v>1100</v>
       </c>
-      <c r="F87" s="45">
-        <v>9950</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="46">
+      <c r="H87" s="63" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="42">
         <v>64</v>
       </c>
-      <c r="C88" s="47">
+      <c r="C88" s="43">
         <v>6</v>
       </c>
-      <c r="D88" s="48" t="s">
+      <c r="D88" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E88" s="47">
+      <c r="E88" s="64">
+        <v>9920</v>
+      </c>
+      <c r="F88" s="44" t="s">
+        <v>381</v>
+      </c>
+      <c r="G88" s="43">
         <v>1600</v>
       </c>
-      <c r="F88" s="49">
-        <v>9920</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="46">
+      <c r="H88" s="65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="42">
         <v>64</v>
       </c>
-      <c r="C89" s="47">
+      <c r="C89" s="43">
         <v>6</v>
       </c>
-      <c r="D89" s="48" t="s">
+      <c r="D89" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E89" s="47">
+      <c r="E89" s="64">
+        <v>9890</v>
+      </c>
+      <c r="F89" s="44" t="s">
+        <v>382</v>
+      </c>
+      <c r="G89" s="43">
         <v>2000</v>
       </c>
-      <c r="F89" s="49">
-        <v>9890</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="50">
+      <c r="H89" s="65" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="45">
         <v>64</v>
       </c>
-      <c r="C90" s="51">
+      <c r="C90" s="46">
         <v>6</v>
       </c>
-      <c r="D90" s="52" t="s">
+      <c r="D90" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E90" s="51">
+      <c r="E90" s="66">
+        <v>9860</v>
+      </c>
+      <c r="F90" s="47" t="s">
+        <v>383</v>
+      </c>
+      <c r="G90" s="46">
         <v>2600</v>
       </c>
-      <c r="F90" s="53">
-        <v>9860</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H90" s="67" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="30">
         <v>68</v>
       </c>
@@ -3004,133 +4212,181 @@
       <c r="D91" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="31">
+      <c r="E91" s="56">
+        <v>9830</v>
+      </c>
+      <c r="F91" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="G91" s="31">
         <v>1200</v>
       </c>
-      <c r="F91" s="33">
-        <v>9830</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="34">
+      <c r="H91" s="57" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="33">
         <v>68</v>
       </c>
-      <c r="C92" s="35">
+      <c r="C92" s="34">
         <v>6</v>
       </c>
-      <c r="D92" s="36" t="s">
+      <c r="D92" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E92" s="35">
+      <c r="E92" s="58">
+        <v>9800</v>
+      </c>
+      <c r="F92" s="35" t="s">
+        <v>385</v>
+      </c>
+      <c r="G92" s="34">
         <v>1700</v>
       </c>
-      <c r="F92" s="37">
-        <v>9800</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="34">
+      <c r="H92" s="59" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="33">
         <v>68</v>
       </c>
-      <c r="C93" s="35">
+      <c r="C93" s="34">
         <v>6</v>
       </c>
-      <c r="D93" s="36" t="s">
+      <c r="D93" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E93" s="35">
+      <c r="E93" s="58">
+        <v>9770</v>
+      </c>
+      <c r="F93" s="35" t="s">
+        <v>386</v>
+      </c>
+      <c r="G93" s="34">
         <v>2200</v>
       </c>
-      <c r="F93" s="37">
-        <v>9770</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="38">
+      <c r="H93" s="59" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="36">
         <v>68</v>
       </c>
-      <c r="C94" s="39">
+      <c r="C94" s="37">
         <v>6</v>
       </c>
-      <c r="D94" s="40" t="s">
+      <c r="D94" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E94" s="39">
+      <c r="E94" s="60">
+        <v>9740</v>
+      </c>
+      <c r="F94" s="38" t="s">
+        <v>387</v>
+      </c>
+      <c r="G94" s="37">
         <v>2700</v>
       </c>
-      <c r="F94" s="41">
-        <v>9740</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="42">
+      <c r="H94" s="61" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="39">
         <v>72</v>
       </c>
-      <c r="C95" s="43">
+      <c r="C95" s="40">
         <v>6</v>
       </c>
-      <c r="D95" s="44" t="s">
+      <c r="D95" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="43">
+      <c r="E95" s="62">
+        <v>9710</v>
+      </c>
+      <c r="F95" s="41" t="s">
+        <v>388</v>
+      </c>
+      <c r="G95" s="40">
         <v>1300</v>
       </c>
-      <c r="F95" s="45">
-        <v>9710</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="46">
+      <c r="H95" s="63" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="42">
         <v>72</v>
       </c>
-      <c r="C96" s="47">
+      <c r="C96" s="43">
         <v>6</v>
       </c>
-      <c r="D96" s="48" t="s">
+      <c r="D96" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E96" s="47">
+      <c r="E96" s="64">
+        <v>9680</v>
+      </c>
+      <c r="F96" s="44" t="s">
+        <v>389</v>
+      </c>
+      <c r="G96" s="43">
         <v>1800</v>
       </c>
-      <c r="F96" s="49">
-        <v>9680</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="46">
+      <c r="H96" s="65" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="42">
         <v>72</v>
       </c>
-      <c r="C97" s="47">
+      <c r="C97" s="43">
         <v>6</v>
       </c>
-      <c r="D97" s="48" t="s">
+      <c r="D97" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E97" s="47">
+      <c r="E97" s="64">
+        <v>9650</v>
+      </c>
+      <c r="F97" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="G97" s="43">
         <v>2300</v>
       </c>
-      <c r="F97" s="49">
-        <v>9650</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="50">
+      <c r="H97" s="65" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="45">
         <v>72</v>
       </c>
-      <c r="C98" s="51">
+      <c r="C98" s="46">
         <v>6</v>
       </c>
-      <c r="D98" s="52" t="s">
+      <c r="D98" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E98" s="51">
+      <c r="E98" s="66">
+        <v>9620</v>
+      </c>
+      <c r="F98" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="G98" s="46">
         <v>2800</v>
       </c>
-      <c r="F98" s="53">
-        <v>9620</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H98" s="67" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="30">
         <v>76</v>
       </c>
@@ -3140,130 +4396,178 @@
       <c r="D99" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E99" s="31">
+      <c r="E99" s="56">
+        <v>9590</v>
+      </c>
+      <c r="F99" s="32" t="s">
+        <v>392</v>
+      </c>
+      <c r="G99" s="31">
         <v>1000</v>
       </c>
-      <c r="F99" s="33">
-        <v>9590</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" s="34">
+      <c r="H99" s="57" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="33">
         <v>76</v>
       </c>
-      <c r="C100" s="35">
+      <c r="C100" s="34">
         <v>6</v>
       </c>
-      <c r="D100" s="36" t="s">
+      <c r="D100" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E100" s="35">
+      <c r="E100" s="58">
+        <v>9560</v>
+      </c>
+      <c r="F100" s="35" t="s">
+        <v>393</v>
+      </c>
+      <c r="G100" s="34">
         <v>1500</v>
       </c>
-      <c r="F100" s="37">
-        <v>9560</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" s="34">
+      <c r="H100" s="59" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="33">
         <v>76</v>
       </c>
-      <c r="C101" s="35">
+      <c r="C101" s="34">
         <v>6</v>
       </c>
-      <c r="D101" s="36" t="s">
+      <c r="D101" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="35">
+      <c r="E101" s="58">
+        <v>9530</v>
+      </c>
+      <c r="F101" s="35" t="s">
+        <v>394</v>
+      </c>
+      <c r="G101" s="34">
         <v>2000</v>
       </c>
-      <c r="F101" s="37">
-        <v>9530</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="38">
+      <c r="H101" s="59" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="36">
         <v>76</v>
       </c>
-      <c r="C102" s="39">
+      <c r="C102" s="37">
         <v>6</v>
       </c>
-      <c r="D102" s="40" t="s">
+      <c r="D102" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E102" s="39">
+      <c r="E102" s="60">
+        <v>9500</v>
+      </c>
+      <c r="F102" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="G102" s="37">
         <v>2500</v>
       </c>
-      <c r="F102" s="41">
-        <v>9500</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" s="42">
+      <c r="H102" s="61" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="39">
         <v>80</v>
       </c>
-      <c r="C103" s="43">
+      <c r="C103" s="40">
         <v>6</v>
       </c>
-      <c r="D103" s="44" t="s">
+      <c r="D103" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E103" s="43">
+      <c r="E103" s="62">
+        <v>9470</v>
+      </c>
+      <c r="F103" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="G103" s="40">
         <v>1100</v>
       </c>
-      <c r="F103" s="45">
-        <v>9470</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" s="46">
+      <c r="H103" s="63" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="42">
         <v>80</v>
       </c>
-      <c r="C104" s="47">
+      <c r="C104" s="43">
         <v>6</v>
       </c>
-      <c r="D104" s="48" t="s">
+      <c r="D104" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E104" s="47">
+      <c r="E104" s="64">
+        <v>9440</v>
+      </c>
+      <c r="F104" s="44" t="s">
+        <v>397</v>
+      </c>
+      <c r="G104" s="43">
         <v>1600</v>
       </c>
-      <c r="F104" s="49">
-        <v>9440</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="46">
+      <c r="H104" s="65" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="42">
         <v>80</v>
       </c>
-      <c r="C105" s="47">
+      <c r="C105" s="43">
         <v>6</v>
       </c>
-      <c r="D105" s="48" t="s">
+      <c r="D105" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E105" s="47">
+      <c r="E105" s="64">
+        <v>9410</v>
+      </c>
+      <c r="F105" s="44" t="s">
+        <v>398</v>
+      </c>
+      <c r="G105" s="43">
         <v>2000</v>
       </c>
-      <c r="F105" s="49">
-        <v>9410</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="50">
+      <c r="H105" s="65" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="45">
         <v>80</v>
       </c>
-      <c r="C106" s="51">
+      <c r="C106" s="46">
         <v>6</v>
       </c>
-      <c r="D106" s="52" t="s">
+      <c r="D106" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E106" s="51">
+      <c r="E106" s="66">
+        <v>9380</v>
+      </c>
+      <c r="F106" s="47" t="s">
+        <v>399</v>
+      </c>
+      <c r="G106" s="46">
         <v>2600</v>
       </c>
-      <c r="F106" s="53">
-        <v>9380</v>
+      <c r="H106" s="67" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -3956,105 +5260,105 @@
       <c r="E3" s="31">
         <v>1000</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="48">
         <v>5500</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="52" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="46">
+      <c r="B4" s="42">
         <v>7</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="43">
         <v>1</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="43">
         <v>1600</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="49">
         <v>2450</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="53" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="34">
+      <c r="B5" s="33">
         <v>8</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="34">
         <v>2200</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="56">
+      <c r="G5" s="50">
         <v>5600</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="53" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="46">
+      <c r="B6" s="42">
         <v>9</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="43">
         <v>2800</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="G6" s="55">
+      <c r="G6" s="49">
         <v>1450</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="53" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38">
+      <c r="B7" s="36">
         <v>10</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="37">
         <v>2000</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="54" t="s">
         <v>188</v>
       </c>
-      <c r="G7" s="57">
+      <c r="G7" s="51">
         <v>6600</v>
       </c>
-      <c r="H7" s="60" t="s">
+      <c r="H7" s="54" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4070,7 +5374,7 @@
   <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4336,6 +5640,9 @@
       <c r="C16" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="E16" s="68" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="5">

</xml_diff>